<commit_message>
Dispatcher - Adicionar itens á fila
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Documents\UiPath\_UDEMY\Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E999EED-F60B-4EB2-BEF1-87805385032D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC3208C-145C-4B24-8962-9EEF6AF0689E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -159,9 +159,6 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
-  </si>
-  <si>
     <t>ACME_URL</t>
   </si>
   <si>
@@ -178,6 +175,12 @@
   </si>
   <si>
     <t>https://acme-test.uipath.com/invoices/search-by-vendor</t>
+  </si>
+  <si>
+    <t>FilaFaturas</t>
+  </si>
+  <si>
+    <t>Bots</t>
   </si>
 </sst>
 </file>
@@ -230,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -240,7 +243,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,7 +560,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -608,7 +610,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -618,7 +620,9 @@
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>32</v>
       </c>
@@ -637,26 +641,26 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
         <v>49</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>